<commit_message>
query fixed. Successfully tested from start to end
</commit_message>
<xml_diff>
--- a/storage/store.xlsx
+++ b/storage/store.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="customer" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="item" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="fact" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="facts" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -168,13 +168,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -200,7 +204,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -308,7 +312,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -392,13 +396,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -553,6 +557,9 @@
       <c r="D11" s="1" t="n">
         <v>25</v>
       </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
query working with UI
</commit_message>
<xml_diff>
--- a/storage/store.xlsx
+++ b/storage/store.xlsx
@@ -168,17 +168,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -200,11 +196,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -312,7 +308,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -396,13 +392,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -557,9 +553,6 @@
       <c r="D11" s="1" t="n">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>